<commit_message>
new build for website update
</commit_message>
<xml_diff>
--- a/StructureDefinition-cbs-cause-of-death.xlsx
+++ b/StructureDefinition-cbs-cause-of-death.xlsx
@@ -3514,7 +3514,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
         <v>189</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>44</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>45</v>

</xml_diff>